<commit_message>
Add pipfile and update README.md
</commit_message>
<xml_diff>
--- a/MainScraper/webpages (1).xlsx
+++ b/MainScraper/webpages (1).xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01_MyFolders\01_FreelancingProjects\01_Freelancer\WebScraper\MainScraper\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="5"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Websites" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Page Results'!$A$1:$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Websites!$S$1:$V$1390</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -6686,6 +6691,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -6979,7 +6987,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6992,9 +7000,7 @@
   </sheetPr>
   <dimension ref="A1:AB1390"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -22062,7 +22068,7 @@
     </row>
     <row r="834" spans="18:21">
       <c r="R834" t="str">
-        <f t="shared" ref="R834:R897" si="13">CONCATENATE("https://www.",S834)</f>
+        <f t="shared" ref="R834:R868" si="13">CONCATENATE("https://www.",S834)</f>
         <v>https://www.blackfridayentufarmacia.es</v>
       </c>
       <c r="S834" s="13" t="s">
@@ -26438,7 +26444,7 @@
     </row>
     <row r="1126" spans="18:21">
       <c r="R1126" t="str">
-        <f t="shared" ref="R1126:R1189" si="18">CONCATENATE("https://www.",S1126)</f>
+        <f t="shared" ref="R1126:R1136" si="18">CONCATENATE("https://www.",S1126)</f>
         <v>https://www.calpoltablets.co.za</v>
       </c>
       <c r="S1126" s="13" t="s">
@@ -29494,7 +29500,7 @@
     </row>
     <row r="1330" spans="18:21">
       <c r="R1330" t="str">
-        <f t="shared" ref="R1330:R1393" si="22">CONCATENATE("https://www.",S1330)</f>
+        <f t="shared" ref="R1330:R1390" si="22">CONCATENATE("https://www.",S1330)</f>
         <v>https://www.preoccupazioneinmeno.it</v>
       </c>
       <c r="S1330" s="13" t="s">
@@ -30911,7 +30917,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:A655"/>
   <sheetViews>
-    <sheetView topLeftCell="A620" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
@@ -34208,7 +34214,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G21" sqref="G21"/>
+      <selection pane="topRight" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -34241,7 +34247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>

</xml_diff>